<commit_message>
Updated script 'prepare_dataset_for_experiment.m' - updated script to read the 'EbmPredictions' column - added in data/final/ the training_test_dataset_compact.mat
</commit_message>
<xml_diff>
--- a/data/final/Lx_Dataset_EstuarIO_Final_Training_Test_Data.xlsx
+++ b/data/final/Lx_Dataset_EstuarIO_Final_Training_Test_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4_CMCC\Progetti\6_EstuarIO\Experiment\data\final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180116A6-0FFE-4B4B-9E12-95B69C37A2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3881152B-D27E-42D5-A4E2-667CEF045D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="4455" windowWidth="19695" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GORO" sheetId="1" r:id="rId1"/>
@@ -458,14 +458,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="7" style="2" bestFit="1" customWidth="1"/>
@@ -3688,7 +3688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>

</xml_diff>